<commit_message>
Implement migration of Queues and Queue Items
</commit_message>
<xml_diff>
--- a/Workbooks/EN/FolderMigration.xlsx
+++ b/Workbooks/EN/FolderMigration.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Workbooks\EN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD6D9FE-376C-4723-BEFE-3E552B5D8DE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED91A750-085D-4DCF-B7EB-2CD421A53319}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5086,7 +5086,7 @@
       <formula1>"Custom Roles,Inherit from tenant"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{AA080958-500E-4C7B-8D0B-FF1C0095F3C4}">
-      <formula1>"Migrate All Items,Migrate New Items,Migrate Queue Definition But Not Queue Items,Do Not Migrate Queue"</formula1>
+      <formula1>"Migrate Queue Definition and New Items,Migrate Queue Definition But Not Queue Items,Do Not Migrate Queue"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Deactivate instead of deleting during migration to Modern Folders
</commit_message>
<xml_diff>
--- a/Workbooks/EN/FolderMigration.xlsx
+++ b/Workbooks/EN/FolderMigration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Workbooks\EN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCBACE82-1C70-4902-AC9D-020683BF4D92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC678372-A7BF-4B6F-A9CA-4B2D12D4F830}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Processes" sheetId="4" r:id="rId1"/>
@@ -8327,7 +8327,7 @@
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Migration Policy" error="Please select a supported Robot Migration Policy." sqref="C2:C1048576" xr:uid="{F72CD099-50BD-4BCC-A62D-6804C9FB3278}">
-      <formula1>"Overwrite Execution Settings,Delete Classic Robot,Overwrite Execution Settings And Delete Classic Robot, Do Not Overwrite Execution Settings Nor Delete Classic Robot"</formula1>
+      <formula1>"Overwrite Execution Settings,Deactivate Classic Robot,Overwrite Execution Settings And Deactivate Classic Robot,Do Not Overwrite Execution Settings Nor Deactivate Classic Robot"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Roles Assignment Model" error="Please select a supported Roles Assignment model." sqref="B202:B1048576" xr:uid="{52C24A50-8937-4451-8BB5-47310592CBC5}">
       <formula1>"Custom Roles,Inherit from tenant"</formula1>

</xml_diff>